<commit_message>
Add deref too fallback
</commit_message>
<xml_diff>
--- a/sample/test/deref/deref_template.xlsx
+++ b/sample/test/deref/deref_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narongdejsrn/Projects/exco/sample/test/deref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF5FC68-9A15-6747-BC36-9CF8A901BAF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E5DC2B-12C5-CF4A-AE42-0BDA2E5ABF19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29680" yWindow="6240" windowWidth="25600" windowHeight="15000" xr2:uid="{CD521CE3-CB81-4AD2-AA9F-DD3573C62CCF}"/>
+    <workbookView xWindow="21240" yWindow="5460" windowWidth="25600" windowHeight="15000" xr2:uid="{CD521CE3-CB81-4AD2-AA9F-DD3573C62CCF}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet" sheetId="2" r:id="rId1"/>
@@ -79,7 +79,17 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">parser: date
+          <t xml:space="preserve">fallback: &lt;&lt;A5&gt;&gt;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">parser: int
 </t>
         </r>
         <r>
@@ -469,7 +479,7 @@
   <dimension ref="A2:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Turn deref_text into DerefCell and add key deref
</commit_message>
<xml_diff>
--- a/sample/test/deref/deref_template.xlsx
+++ b/sample/test/deref/deref_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narongdejsrn/Projects/exco/sample/test/deref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E5DC2B-12C5-CF4A-AE42-0BDA2E5ABF19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FD548A-9EFC-474C-900D-D475A31A97AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21240" yWindow="5460" windowWidth="25600" windowHeight="15000" xr2:uid="{CD521CE3-CB81-4AD2-AA9F-DD3573C62CCF}"/>
   </bookViews>
@@ -28,6 +28,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Microsoft Office User</author>
+    <author>Narongdej Sarnsuwan</author>
   </authors>
   <commentList>
     <comment ref="B2" authorId="0" shapeId="0" xr:uid="{5E40A18F-FF1A-FE49-A81B-4320C388A656}">
@@ -80,6 +81,69 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">fallback: &lt;&lt;A5&gt;&gt;
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">parser: int
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>--}}</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{89840BA3-E6FE-0E42-B314-A6A0690BF67F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Narongdej Sarnsuwan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">{{--
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">key: &lt;&lt;A1&gt;&gt;_wealth
 </t>
         </r>
         <r>
@@ -108,9 +172,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>sum_val</t>
+  </si>
+  <si>
+    <t>wealth</t>
+  </si>
+  <si>
+    <t>awesome</t>
   </si>
 </sst>
 </file>
@@ -177,6 +247,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDBE698-D470-46AC-96B1-DE0D5151A06B}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -487,6 +561,11 @@
     <col min="2" max="2" width="9.83203125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
@@ -495,6 +574,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>200</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>

<commit_message>
Turn deref into a factory
</commit_message>
<xml_diff>
--- a/sample/test/deref/deref_template.xlsx
+++ b/sample/test/deref/deref_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/narongdejsrn/Projects/exco/sample/test/deref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FD548A-9EFC-474C-900D-D475A31A97AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F782F5-8E05-144B-922D-61A1132C3041}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="21240" yWindow="5460" windowWidth="25600" windowHeight="15000" xr2:uid="{CD521CE3-CB81-4AD2-AA9F-DD3573C62CCF}"/>
   </bookViews>
@@ -167,12 +167,122 @@
         </r>
       </text>
     </comment>
+    <comment ref="B4" authorId="1" shapeId="0" xr:uid="{BE5AE63E-01F6-6D48-A6D9-704EA85292C6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>Microsoft Office User:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>{{--</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>key: &lt;&lt;A4&gt;&gt;</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>fallback: 0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">parser: int
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">deref: no
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>--}}</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>sum_val</t>
   </si>
@@ -182,12 +292,15 @@
   <si>
     <t>awesome</t>
   </si>
+  <si>
+    <t>no_deref</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,6 +320,25 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -247,10 +379,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -550,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBDBE698-D470-46AC-96B1-DE0D5151A06B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -582,6 +710,14 @@
         <v>200</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>